<commit_message>
Completed fixing % of parent row total bug and added tests.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTables/PivotTableMixedDataFieldFunctionTypes.xlsx
+++ b/EPPlusTest/Workbooks/PivotTables/PivotTableMixedDataFieldFunctionTypes.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\PivotTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54172A30-F31A-411A-A463-F32BC24DFD94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DDDCCF-D847-4990-8807-1B7DFB92AB66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="1" xr2:uid="{EE242619-6CE1-4DE4-AA87-2BE8671EA6F5}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="130">
   <si>
     <t>No.</t>
   </si>
@@ -378,16 +378,52 @@
     <t>Total Product of Net Change</t>
   </si>
   <si>
-    <t>Product of Balance at End Date</t>
-  </si>
-  <si>
-    <t>Total Product of Balance at End Date</t>
-  </si>
-  <si>
-    <t>Sum of Net Change (Prior Year)</t>
-  </si>
-  <si>
-    <t>Total Sum of Net Change (Prior Year)</t>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Total Count of Indentation</t>
+  </si>
+  <si>
+    <t>Count of Indentation</t>
+  </si>
+  <si>
+    <t>Total Average of Income/Balance</t>
+  </si>
+  <si>
+    <t>Average of Income/Balance</t>
   </si>
 </sst>
 </file>
@@ -1164,49 +1200,19 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4D5D907-B3EC-40F9-BD55-3ED3A8BBE92F}" name="PivotTable3" cacheId="4" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
-  <location ref="A40:N52" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C37A20F5-5BBA-4F43-916D-CC11843CCCF9}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="A40:L66" firstHeaderRow="1" firstDataRow="3" firstDataCol="3"/>
   <pivotFields count="16">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="27">
-        <item x="21"/>
-        <item x="25"/>
-        <item x="4"/>
-        <item x="9"/>
-        <item x="7"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="16"/>
-        <item x="18"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="19"/>
-        <item x="26"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="17"/>
-        <item x="15"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item x="12"/>
-        <item x="3"/>
-        <item x="20"/>
-        <item x="11"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="3">
         <item x="0"/>
         <item x="2"/>
         <item x="1"/>
       </items>
     </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField axis="axisCol" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="2">
         <item x="0"/>
         <item x="1"/>
@@ -1220,7 +1226,7 @@
       </items>
     </pivotField>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField axis="axisRow" compact="0" numFmtId="14" outline="0" showAll="0" defaultSubtotal="0">
       <items count="14">
         <item x="0"/>
         <item x="1"/>
@@ -1238,22 +1244,9 @@
         <item x="13"/>
       </items>
     </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="10">
-        <item x="0"/>
-        <item x="8"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="9"/>
-      </items>
-    </pivotField>
-    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
       </items>
@@ -1274,49 +1267,16 @@
         <item x="1"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="14">
-        <item x="13"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="0"/>
-        <item x="8"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="7"/>
-        <item x="9"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="10"/>
-        <item x="6"/>
-        <item x="2"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="13">
-        <item x="12"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="6"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="2"/>
-        <item x="7"/>
-      </items>
-    </pivotField>
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="6">
         <item sd="0" x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
         <item sd="0" x="5"/>
       </items>
     </pivotField>
@@ -1336,78 +1296,139 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="2">
-    <field x="14"/>
+  <rowFields count="3">
+    <field x="6"/>
+    <field x="2"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="10">
+  <rowItems count="24">
     <i>
       <x v="1"/>
       <x/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
     </i>
     <i r="1">
       <x v="2"/>
+      <x v="2"/>
     </i>
     <i>
       <x v="2"/>
+      <x v="1"/>
       <x/>
     </i>
     <i r="1">
       <x v="2"/>
+      <x/>
     </i>
     <i>
       <x v="3"/>
       <x/>
+      <x/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+      <x v="2"/>
     </i>
     <i r="1">
       <x v="1"/>
+      <x v="2"/>
     </i>
     <i>
-      <x v="4"/>
+      <x v="6"/>
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x/>
       <x/>
     </i>
     <i r="1">
       <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x v="1"/>
+      <x/>
     </i>
     <i r="1">
       <x v="2"/>
+      <x/>
+    </i>
+    <i>
+      <x v="9"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="10"/>
+      <x/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="11"/>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i>
+      <x v="12"/>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
   <colFields count="2">
+    <field x="3"/>
     <field x="-2"/>
-    <field x="2"/>
   </colFields>
-  <colItems count="12">
+  <colItems count="9">
     <i>
       <x/>
       <x/>
     </i>
-    <i r="1">
+    <i r="1" i="1">
       <x v="1"/>
     </i>
-    <i r="1">
+    <i r="1" i="2">
       <x v="2"/>
     </i>
-    <i i="1">
+    <i>
       <x v="1"/>
       <x/>
     </i>
     <i r="1" i="1">
       <x v="1"/>
     </i>
-    <i r="1" i="1">
-      <x v="2"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="2">
-      <x v="1"/>
-    </i>
     <i r="1" i="2">
       <x v="2"/>
     </i>
@@ -1422,21 +1443,21 @@
     </i>
   </colItems>
   <dataFields count="3">
-    <dataField name="Count of Net Change" fld="10" subtotal="count" baseField="3" baseItem="1" numFmtId="10">
+    <dataField name="Count of Indentation" fld="7" subtotal="count" baseField="0" baseItem="0" numFmtId="10">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
           <x14:dataField pivotShowAs="percentOfParentRow"/>
         </ext>
       </extLst>
     </dataField>
-    <dataField name="Product of Balance at End Date" fld="11" subtotal="product" baseField="3" baseItem="1" numFmtId="10">
+    <dataField name="Average of Income/Balance" fld="9" subtotal="average" baseField="0" baseItem="0" numFmtId="10">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
           <x14:dataField pivotShowAs="percentOfParentRow"/>
         </ext>
       </extLst>
     </dataField>
-    <dataField name="Sum of Net Change (Prior Year)" fld="12" baseField="3" baseItem="0" numFmtId="10">
+    <dataField name="Product of Net Change" fld="10" subtotal="product" baseField="0" baseItem="0" numFmtId="10">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{E15A36E0-9728-4e99-A89B-3F7291B0FE68}">
           <x14:dataField pivotShowAs="percentOfParentRow"/>
@@ -1457,7 +1478,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF392B1D-EF0B-4234-9317-EE0AB24B591D}" name="PivotTable2" cacheId="4" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AF392B1D-EF0B-4234-9317-EE0AB24B591D}" name="PivotTable2" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:N36" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -1694,7 +1715,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41B8CC38-7DCD-4F2C-9876-3C44E2816BD8}" name="PivotTable1" cacheId="4" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41B8CC38-7DCD-4F2C-9876-3C44E2816BD8}" name="PivotTable1" cacheId="1" dataOnRows="1" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A1:K15" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
   <pivotFields count="16">
     <pivotField compact="0" outline="0" showAll="0" defaultSubtotal="0"/>
@@ -3524,22 +3545,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52C5FAE-589A-4D62-88AD-05AA44BCB8EF}">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I28" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.77734375" bestFit="1" customWidth="1"/>
@@ -4590,222 +4614,162 @@
       <c r="N36" s="4"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C41" t="s">
-        <v>94</v>
-      </c>
-      <c r="F41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I41" t="s">
-        <v>116</v>
+      <c r="D41" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" t="s">
+        <v>91</v>
+      </c>
+      <c r="J41" t="s">
+        <v>126</v>
+      </c>
+      <c r="K41" t="s">
+        <v>128</v>
       </c>
       <c r="L41" t="s">
-        <v>96</v>
-      </c>
-      <c r="M41" t="s">
-        <v>115</v>
-      </c>
-      <c r="N41" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" t="s">
+        <v>129</v>
+      </c>
+      <c r="F42" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" t="s">
+        <v>127</v>
+      </c>
+      <c r="H42" t="s">
+        <v>129</v>
+      </c>
+      <c r="I42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" t="s">
         <v>16</v>
       </c>
-      <c r="D42" t="s">
-        <v>26</v>
-      </c>
-      <c r="E42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" t="s">
-        <v>26</v>
-      </c>
-      <c r="H42" t="s">
-        <v>22</v>
-      </c>
-      <c r="I42" t="s">
-        <v>16</v>
-      </c>
-      <c r="J42" t="s">
-        <v>26</v>
-      </c>
-      <c r="K42" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="E43" s="4">
-        <v>0</v>
-      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4">
-        <v>0</v>
-      </c>
+      <c r="G43" s="4">
+        <v>1</v>
+      </c>
+      <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4">
-        <v>0</v>
-      </c>
-      <c r="L43" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4">
-        <v>0</v>
-      </c>
+      <c r="J43" s="4">
+        <v>1</v>
+      </c>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4">
+        <v>1</v>
+      </c>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4">
+        <v>1</v>
+      </c>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D44" s="4">
-        <v>0</v>
-      </c>
-      <c r="E44" s="4">
-        <v>1</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4">
-        <v>1</v>
-      </c>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4">
-        <v>1</v>
-      </c>
-      <c r="L44" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="4">
-        <v>0</v>
-      </c>
-      <c r="D45" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E45" s="4">
-        <v>0</v>
-      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4">
-        <v>1.2785597615492182E-7</v>
-      </c>
-      <c r="H45" s="4">
-        <v>0</v>
-      </c>
-      <c r="I45" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4">
+        <v>1</v>
+      </c>
       <c r="J45" s="4">
-        <v>4.486239850794548</v>
-      </c>
-      <c r="K45" s="4">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K45" s="4"/>
       <c r="L45" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4">
-        <v>3.8614613196294072</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="B46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="4">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="C46" t="s">
+        <v>17</v>
       </c>
       <c r="D46" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E46" s="4">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="4">
-        <v>-1.4806972756871448E-7</v>
-      </c>
-      <c r="H46" s="4">
-        <v>1</v>
-      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4">
-        <v>-3.486239850794548</v>
-      </c>
-      <c r="K46" s="4">
-        <v>1</v>
-      </c>
-      <c r="L46" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4">
-        <v>-2.8614613196294072</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>90</v>
-      </c>
       <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D47" s="4">
-        <v>1</v>
-      </c>
-      <c r="E47" s="4">
-        <v>1</v>
-      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4">
         <v>1</v>
@@ -4816,160 +4780,123 @@
         <v>1</v>
       </c>
       <c r="K47" s="4"/>
-      <c r="L47" s="4">
-        <v>1</v>
-      </c>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4">
-        <v>1</v>
-      </c>
+      <c r="L47" s="4"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="B48" t="s">
-        <v>33</v>
-      </c>
-      <c r="C48" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D48" s="4">
-        <v>0</v>
-      </c>
-      <c r="E48" s="4">
-        <v>0</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" s="4"/>
-      <c r="L48" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>89</v>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B49" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="4">
-        <v>0</v>
-      </c>
       <c r="D49" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="4">
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4">
-        <v>5.2694566704328883E-7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4">
+        <v>1</v>
+      </c>
+      <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4">
-        <v>1.0997636673163009</v>
-      </c>
-      <c r="K49" s="4">
-        <v>-2.7851546380781373</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K49" s="4"/>
       <c r="L49" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4">
-        <v>2.2706112499749018</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="B50" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="4">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
       </c>
       <c r="D50" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E50" s="4">
-        <v>0.14285714285714285</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="4">
-        <v>1.2785597615492182E-7</v>
-      </c>
+      <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4">
-        <v>-9.9763667316301041E-2</v>
-      </c>
-      <c r="K50" s="4">
-        <v>0</v>
-      </c>
-      <c r="L50" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4">
-        <v>-0.12983072137822382</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="4">
-        <v>0</v>
-      </c>
-      <c r="D51" s="4">
-        <v>0</v>
-      </c>
-      <c r="E51" s="4">
-        <v>0.42857142857142855</v>
-      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
+      <c r="I51" s="4">
+        <v>1</v>
+      </c>
       <c r="J51" s="4">
-        <v>0</v>
-      </c>
-      <c r="K51" s="4">
-        <v>3.7851546380781373</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K51" s="4"/>
       <c r="L51" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4">
-        <v>-1.1407805285966779</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>86</v>
-      </c>
-      <c r="C52" s="4">
-        <v>1</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
       </c>
       <c r="D52" s="4">
         <v>1</v>
       </c>
-      <c r="E52" s="4">
-        <v>1</v>
-      </c>
+      <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
@@ -4977,16 +4904,342 @@
       <c r="J52" s="4">
         <v>1</v>
       </c>
-      <c r="K52" s="4">
-        <v>1</v>
-      </c>
-      <c r="L52" s="4">
-        <v>1</v>
-      </c>
-      <c r="M52" s="4"/>
-      <c r="N52" s="4">
-        <v>1</v>
-      </c>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1</v>
+      </c>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4">
+        <v>1</v>
+      </c>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4">
+        <v>1</v>
+      </c>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4">
+        <v>1</v>
+      </c>
+      <c r="J54" s="4">
+        <v>1</v>
+      </c>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="4">
+        <v>1</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4">
+        <v>1</v>
+      </c>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4">
+        <v>1</v>
+      </c>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4">
+        <v>1</v>
+      </c>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4">
+        <v>1</v>
+      </c>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4">
+        <v>1</v>
+      </c>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4">
+        <v>1</v>
+      </c>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4">
+        <v>5.6440027222153937E-6</v>
+      </c>
+      <c r="J59" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4">
+        <v>5.6440027222153937E-6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4">
+        <v>2.5307392446239383E-6</v>
+      </c>
+      <c r="J60" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4">
+        <v>2.5307392446239383E-6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4">
+        <v>3.6646883457413577E-5</v>
+      </c>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4">
+        <v>3.6646883457413577E-5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4">
+        <v>1.0717106226992383E-5</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4">
+        <v>1.0717106226992383E-5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C63" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="4">
+        <v>1</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4">
+        <v>1</v>
+      </c>
+      <c r="G63" s="4">
+        <v>1</v>
+      </c>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4">
+        <v>1</v>
+      </c>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
+        <v>22</v>
+      </c>
+      <c r="C64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4">
+        <v>0</v>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4">
+        <v>0</v>
+      </c>
+      <c r="J64" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4">
+        <v>1</v>
+      </c>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4">
+        <v>1</v>
+      </c>
+      <c r="J65" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D66" s="4">
+        <v>1</v>
+      </c>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4">
+        <v>1</v>
+      </c>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4">
+        <v>1</v>
+      </c>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>